<commit_message>
Added percent change for print statement comparing previous to current price
</commit_message>
<xml_diff>
--- a/excelworkbooktest/TD Ameritrade stonks.xlsx
+++ b/excelworkbooktest/TD Ameritrade stonks.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="980" yWindow="1000" windowWidth="24620" windowHeight="10710" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6620" yWindow="2850" windowWidth="28800" windowHeight="15460" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2021 Portfolio" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Portfolio" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2021 Dividends" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="$Contributed$" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="ETH" sheetId="4" state="visible" r:id="rId4"/>
@@ -385,7 +385,7 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,13 +398,177 @@
     <cellStyle name="Heading 4" xfId="7" builtinId="19"/>
     <cellStyle name="Heading 1" xfId="8" builtinId="16"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.3999450666829432"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE20000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border>
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -437,184 +601,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border>
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.1498764000366222"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.5999633777886288"/>
         </patternFill>
       </fill>
@@ -636,7 +622,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1">
-      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -714,23 +700,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table4" displayName="Table4" ref="A4:G8" headerRowCount="1" totalsRowShown="0">
   <autoFilter ref="A4:G8"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Symbol" dataDxfId="14">
+    <tableColumn id="1" name="Symbol" dataDxfId="8">
       <calculatedColumnFormula array="1">IFERROR(INDEX(Transactions!$B$2:$B$200,MATCH(0,COUNTIF($A$4:A4,Transactions!$B$2:$B$200),0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Shares" dataDxfId="13">
+    <tableColumn id="2" name="Shares" dataDxfId="7">
       <calculatedColumnFormula>IF(A5="","",SUMIFS(Transactions!$E$2:$E$200,Transactions!$B$2:$B$200,A5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Money Invested" dataDxfId="12">
+    <tableColumn id="3" name="Money Invested" dataDxfId="6">
       <calculatedColumnFormula>IF(A5="","",SUMIFS(Transactions!F2:F200,Transactions!B2:B200,A5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Mkt Value" dataDxfId="11">
+    <tableColumn id="4" name="Mkt Value" dataDxfId="5">
       <calculatedColumnFormula>IF(A5="","",SUM(F5*B5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Percent Change" dataDxfId="10">
+    <tableColumn id="5" name="Percent Change" dataDxfId="4">
       <calculatedColumnFormula>IF(A5="","",SUM(D5-C5) / C5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Current Share Price" dataDxfId="9"/>
-    <tableColumn id="7" name="Percent of Total Investment" dataDxfId="8"/>
+    <tableColumn id="6" name="Current Share Price" dataDxfId="3"/>
+    <tableColumn id="7" name="Percent of Total Investment" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1005,9 +991,9 @@
   </sheetPr>
   <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -1093,7 +1079,7 @@
         <v/>
       </c>
       <c r="H2" s="43" t="n">
-        <v>33554.48</v>
+        <v>32961.34</v>
       </c>
       <c r="I2" s="26">
         <f>SUM(H2-G2) / G2</f>
@@ -1692,7 +1678,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -1708,8 +1694,8 @@
     <col width="16.453125" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
     <col width="18.81640625" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
     <col width="13.08984375" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
-    <col width="8.7265625" customWidth="1" style="2" min="12" max="54"/>
-    <col width="8.7265625" customWidth="1" style="2" min="55" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="12" max="60"/>
+    <col width="8.7265625" customWidth="1" style="2" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1785,17 +1771,17 @@
         <v/>
       </c>
       <c r="G2" s="49" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="H2" s="28">
         <f>SUM(G2:G13)</f>
         <v/>
       </c>
       <c r="I2" s="28" t="n">
-        <v>33554.48</v>
+        <v>32961.34</v>
       </c>
       <c r="J2" s="29">
-        <f>(I2-D2-H2)/H2</f>
+        <f>(I2-D2-H2)/D2</f>
         <v/>
       </c>
       <c r="K2" s="3" t="n">
@@ -1943,6 +1929,14 @@
       <c r="C16" s="49" t="n"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J2">
+    <cfRule type="expression" priority="2" dxfId="1">
+      <formula>J2 &lt; 0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="1" dxfId="0">
+      <formula>J2 &gt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -2066,10 +2060,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -2115,7 +2109,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5861801114</v>
+        <v>5924152434</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -2124,26 +2118,26 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D2" s="54" t="n">
-        <v>243.73</v>
+          <t>01/11/2022</t>
+        </is>
+      </c>
+      <c r="D2" s="53" t="n">
+        <v>235.71</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" s="54" t="n">
-        <v>1218.65</v>
+        <v>4</v>
+      </c>
+      <c r="F2" s="53" t="n">
+        <v>942.84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5861801112</v>
+        <v>5861801114</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>VOOG</t>
+          <t>VTI</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
@@ -2151,19 +2145,19 @@
           <t>01/04/2022</t>
         </is>
       </c>
-      <c r="D3" s="54" t="n">
-        <v>304.61</v>
+      <c r="D3" s="53" t="n">
+        <v>243.73</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" s="54" t="n">
-        <v>913.83</v>
+        <v>5</v>
+      </c>
+      <c r="F3" s="53" t="n">
+        <v>1218.65</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5640387460</v>
+        <v>5861801112</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -2172,26 +2166,26 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>12/08/2021</t>
-        </is>
-      </c>
-      <c r="D4" s="54" t="n">
-        <v>300.48</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D4" s="53" t="n">
+        <v>304.61</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="54" t="n">
-        <v>300.48</v>
+        <v>3</v>
+      </c>
+      <c r="F4" s="53" t="n">
+        <v>913.83</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5640387455</v>
+        <v>5640387460</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VTI</t>
+          <t>VOOG</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
@@ -2199,23 +2193,23 @@
           <t>12/08/2021</t>
         </is>
       </c>
-      <c r="D5" s="54" t="n">
-        <v>239.57</v>
+      <c r="D5" s="53" t="n">
+        <v>300.48</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" s="54" t="n">
-        <v>958.28</v>
+        <v>1</v>
+      </c>
+      <c r="F5" s="53" t="n">
+        <v>300.48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5640387458</v>
+        <v>5640387455</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>VTI</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
@@ -2223,67 +2217,67 @@
           <t>12/08/2021</t>
         </is>
       </c>
-      <c r="D6" s="54" t="n">
-        <v>430.93</v>
+      <c r="D6" s="53" t="n">
+        <v>239.57</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" s="54" t="n">
-        <v>861.86</v>
+        <v>4</v>
+      </c>
+      <c r="F6" s="53" t="n">
+        <v>958.28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5273771353</v>
+        <v>5640387458</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VTI</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>11/09/2021</t>
-        </is>
-      </c>
-      <c r="D7" s="54" t="n">
-        <v>242.6</v>
+          <t>12/08/2021</t>
+        </is>
+      </c>
+      <c r="D7" s="53" t="n">
+        <v>430.93</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="54" t="n">
-        <v>242.6</v>
+        <v>2</v>
+      </c>
+      <c r="F7" s="53" t="n">
+        <v>861.86</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4710522295</v>
+        <v>5273771353</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>VTI</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>11/08/2021</t>
-        </is>
-      </c>
-      <c r="D8" s="54" t="n">
-        <v>431.45</v>
+          <t>11/09/2021</t>
+        </is>
+      </c>
+      <c r="D8" s="53" t="n">
+        <v>242.6</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
-      </c>
-      <c r="F8" s="54" t="n">
-        <v>1725.8</v>
+        <v>1</v>
+      </c>
+      <c r="F8" s="53" t="n">
+        <v>242.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4499865043</v>
+        <v>4710522295</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -2292,26 +2286,26 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>10/06/2021</t>
-        </is>
-      </c>
-      <c r="D9" s="54" t="n">
-        <v>394.66</v>
+          <t>11/08/2021</t>
+        </is>
+      </c>
+      <c r="D9" s="53" t="n">
+        <v>431.45</v>
       </c>
       <c r="E9" t="n">
         <v>4</v>
       </c>
-      <c r="F9" s="54" t="n">
-        <v>1578.64</v>
+      <c r="F9" s="53" t="n">
+        <v>1725.8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4499865055</v>
+        <v>4499865043</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>VTI</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
@@ -2319,47 +2313,47 @@
           <t>10/06/2021</t>
         </is>
       </c>
-      <c r="D10" s="54" t="n">
-        <v>221.89</v>
+      <c r="D10" s="53" t="n">
+        <v>394.66</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
-      </c>
-      <c r="F10" s="54" t="n">
-        <v>443.78</v>
+        <v>4</v>
+      </c>
+      <c r="F10" s="53" t="n">
+        <v>1578.64</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4327826726</v>
+        <v>4499865055</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>VTI</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>09/08/2021</t>
-        </is>
-      </c>
-      <c r="D11" s="54" t="n">
-        <v>414.54</v>
+          <t>10/06/2021</t>
+        </is>
+      </c>
+      <c r="D11" s="53" t="n">
+        <v>221.89</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
-      </c>
-      <c r="F11" s="54" t="n">
-        <v>1658.16</v>
+        <v>2</v>
+      </c>
+      <c r="F11" s="53" t="n">
+        <v>443.78</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4327826730</v>
+        <v>4327826726</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>VOOG</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
@@ -2367,47 +2361,47 @@
           <t>09/08/2021</t>
         </is>
       </c>
-      <c r="D12" s="54" t="n">
-        <v>284.77</v>
+      <c r="D12" s="53" t="n">
+        <v>414.54</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="54" t="n">
-        <v>284.77</v>
+        <v>4</v>
+      </c>
+      <c r="F12" s="53" t="n">
+        <v>1658.16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4146304071</v>
+        <v>4327826730</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>VTI</t>
+          <t>VOOG</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>08/06/2021</t>
-        </is>
-      </c>
-      <c r="D13" s="54" t="n">
-        <v>228.59</v>
+          <t>09/08/2021</t>
+        </is>
+      </c>
+      <c r="D13" s="53" t="n">
+        <v>284.77</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="54" t="n">
-        <v>228.59</v>
+      <c r="F13" s="53" t="n">
+        <v>284.77</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>4146304066</v>
+        <v>4146304071</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>VOOG</t>
+          <t>VTI</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
@@ -2415,19 +2409,19 @@
           <t>08/06/2021</t>
         </is>
       </c>
-      <c r="D14" s="54" t="n">
-        <v>275.07</v>
+      <c r="D14" s="53" t="n">
+        <v>228.59</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
-      </c>
-      <c r="F14" s="54" t="n">
-        <v>1375.35</v>
+        <v>1</v>
+      </c>
+      <c r="F14" s="53" t="n">
+        <v>228.59</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3933861348</v>
+        <v>4146304066</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -2436,26 +2430,26 @@
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>07/06/2021</t>
-        </is>
-      </c>
-      <c r="D15" s="54" t="n">
-        <v>266.63</v>
+          <t>08/06/2021</t>
+        </is>
+      </c>
+      <c r="D15" s="53" t="n">
+        <v>275.07</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
-      </c>
-      <c r="F15" s="54" t="n">
-        <v>799.89</v>
+        <v>5</v>
+      </c>
+      <c r="F15" s="53" t="n">
+        <v>1375.35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3933861347</v>
+        <v>3933861348</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>VTI</t>
+          <t>VOOG</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
@@ -2463,19 +2457,19 @@
           <t>07/06/2021</t>
         </is>
       </c>
-      <c r="D16" s="54" t="n">
-        <v>225.27</v>
+      <c r="D16" s="53" t="n">
+        <v>266.63</v>
       </c>
       <c r="E16" t="n">
         <v>3</v>
       </c>
-      <c r="F16" s="54" t="n">
-        <v>675.8099999999999</v>
+      <c r="F16" s="53" t="n">
+        <v>799.89</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2690641270</v>
+        <v>3933861347</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -2484,22 +2478,22 @@
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>05/06/2021</t>
-        </is>
-      </c>
-      <c r="D17" s="54" t="n">
-        <v>214.5</v>
+          <t>07/06/2021</t>
+        </is>
+      </c>
+      <c r="D17" s="53" t="n">
+        <v>225.27</v>
       </c>
       <c r="E17" t="n">
         <v>3</v>
       </c>
-      <c r="F17" s="54" t="n">
-        <v>643.5</v>
+      <c r="F17" s="53" t="n">
+        <v>675.8099999999999</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2687060643</v>
+        <v>2690641270</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -2511,47 +2505,47 @@
           <t>05/06/2021</t>
         </is>
       </c>
-      <c r="D18" s="54" t="n">
-        <v>215.78</v>
+      <c r="D18" s="53" t="n">
+        <v>214.5</v>
       </c>
       <c r="E18" t="n">
         <v>3</v>
       </c>
-      <c r="F18" s="54" t="n">
-        <v>647.34</v>
+      <c r="F18" s="53" t="n">
+        <v>643.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2381703970</v>
+        <v>2687060643</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>VOOG</t>
+          <t>VTI</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>04/06/2021</t>
-        </is>
-      </c>
-      <c r="D19" s="54" t="n">
-        <v>242.88</v>
+          <t>05/06/2021</t>
+        </is>
+      </c>
+      <c r="D19" s="53" t="n">
+        <v>215.78</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
-      </c>
-      <c r="F19" s="54" t="n">
-        <v>1214.4</v>
+        <v>3</v>
+      </c>
+      <c r="F19" s="53" t="n">
+        <v>647.34</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2381703962</v>
+        <v>2381703970</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SPY</t>
+          <t>VOOG</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
@@ -2559,47 +2553,47 @@
           <t>04/06/2021</t>
         </is>
       </c>
-      <c r="D20" s="54" t="n">
-        <v>405.83</v>
+      <c r="D20" s="53" t="n">
+        <v>242.88</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
-      </c>
-      <c r="F20" s="54" t="n">
-        <v>1217.49</v>
+        <v>5</v>
+      </c>
+      <c r="F20" s="53" t="n">
+        <v>1214.4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2227844148</v>
+        <v>2381703962</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>VTI</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
-        </is>
-      </c>
-      <c r="D21" s="54" t="n">
-        <v>196.8</v>
+          <t>04/06/2021</t>
+        </is>
+      </c>
+      <c r="D21" s="53" t="n">
+        <v>405.83</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
-      </c>
-      <c r="F21" s="54" t="n">
-        <v>984</v>
+        <v>3</v>
+      </c>
+      <c r="F21" s="53" t="n">
+        <v>1217.49</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2227844145</v>
+        <v>2227844148</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>VOOG</t>
+          <t>VTI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2607,19 +2601,19 @@
           <t>03/05/2021</t>
         </is>
       </c>
-      <c r="D22" s="54" t="n">
-        <v>222.74</v>
+      <c r="D22" s="53" t="n">
+        <v>196.8</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
-      </c>
-      <c r="F22" s="54" t="n">
-        <v>668.22</v>
+        <v>5</v>
+      </c>
+      <c r="F22" s="53" t="n">
+        <v>984</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2116334823</v>
+        <v>2227844145</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2628,26 +2622,26 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>02/16/2021</t>
-        </is>
-      </c>
-      <c r="D23" s="54" t="n">
-        <v>242.6</v>
+          <t>03/05/2021</t>
+        </is>
+      </c>
+      <c r="D23" s="53" t="n">
+        <v>222.74</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
-      </c>
-      <c r="F23" s="54" t="n">
-        <v>2183.4</v>
+        <v>3</v>
+      </c>
+      <c r="F23" s="53" t="n">
+        <v>668.22</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2116334813</v>
+        <v>2116334823</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>VOOG</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2655,37 +2649,61 @@
           <t>02/16/2021</t>
         </is>
       </c>
-      <c r="D24" s="54" t="n">
-        <v>361.05</v>
+      <c r="D24" s="53" t="n">
+        <v>242.6</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
-      </c>
-      <c r="F24" s="54" t="n">
-        <v>3610.5</v>
+        <v>9</v>
+      </c>
+      <c r="F24" s="53" t="n">
+        <v>2183.4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
+        <v>2116334813</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>02/16/2021</t>
+        </is>
+      </c>
+      <c r="D25" s="53" t="n">
+        <v>361.05</v>
+      </c>
+      <c r="E25" t="n">
+        <v>10</v>
+      </c>
+      <c r="F25" s="53" t="n">
+        <v>3610.5</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
         <v>2116334800</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>VTI</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>02/16/2021</t>
         </is>
       </c>
-      <c r="D25" s="54" t="n">
+      <c r="D26" s="53" t="n">
         <v>207.49</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E26" t="n">
         <v>29</v>
       </c>
-      <c r="F25" s="54" t="n">
+      <c r="F26" s="53" t="n">
         <v>6017.21</v>
       </c>
     </row>
@@ -2704,8 +2722,8 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -2767,25 +2785,25 @@
         </is>
       </c>
       <c r="B2" s="54" t="n">
-        <v>236.06</v>
+        <v>220</v>
       </c>
       <c r="C2" s="54" t="n">
-        <v>236.5</v>
+        <v>220.58</v>
       </c>
       <c r="D2" s="54" t="n">
-        <v>236.11</v>
+        <v>228.91</v>
       </c>
       <c r="E2" s="54" t="n">
-        <v>237.19</v>
+        <v>224.62</v>
       </c>
       <c r="F2" s="54" t="n">
-        <v>238.07</v>
+        <v>226.09</v>
       </c>
       <c r="G2" s="54" t="n">
-        <v>235.32</v>
+        <v>220.825</v>
       </c>
       <c r="H2" s="54" t="n">
-        <v>236.11</v>
+        <v>225.37</v>
       </c>
     </row>
     <row r="3">
@@ -2795,25 +2813,25 @@
         </is>
       </c>
       <c r="B3" s="54" t="n">
-        <v>428.23</v>
+        <v>401.4</v>
       </c>
       <c r="C3" s="54" t="n">
-        <v>428.5</v>
+        <v>401.6</v>
       </c>
       <c r="D3" s="54" t="n">
-        <v>428.59</v>
+        <v>402.69</v>
       </c>
       <c r="E3" s="54" t="n">
-        <v>430.21</v>
+        <v>409.71</v>
       </c>
       <c r="F3" s="54" t="n">
-        <v>431.36</v>
+        <v>411.9265</v>
       </c>
       <c r="G3" s="54" t="n">
-        <v>427.2</v>
+        <v>402.66</v>
       </c>
       <c r="H3" s="54" t="n">
-        <v>428.59</v>
+        <v>410.76</v>
       </c>
     </row>
     <row r="4">
@@ -2823,25 +2841,25 @@
         </is>
       </c>
       <c r="B4" s="54" t="n">
-        <v>465.87</v>
+        <v>436.65</v>
       </c>
       <c r="C4" s="54" t="n">
-        <v>466.09</v>
+        <v>436.67</v>
       </c>
       <c r="D4" s="54" t="n">
-        <v>466.09</v>
+        <v>437.98</v>
       </c>
       <c r="E4" s="54" t="n">
-        <v>467.95</v>
+        <v>445.56</v>
       </c>
       <c r="F4" s="54" t="n">
-        <v>469.2</v>
+        <v>448.06</v>
       </c>
       <c r="G4" s="54" t="n">
-        <v>464.65</v>
+        <v>437.95</v>
       </c>
       <c r="H4" s="54" t="n">
-        <v>466.09</v>
+        <v>446.75</v>
       </c>
     </row>
     <row r="5">
@@ -2851,25 +2869,25 @@
         </is>
       </c>
       <c r="B5" s="54" t="n">
-        <v>288</v>
+        <v>262.59</v>
       </c>
       <c r="C5" s="54" t="n">
-        <v>289.95</v>
+        <v>265.89</v>
       </c>
       <c r="D5" s="54" t="n">
-        <v>288.37</v>
+        <v>265.96</v>
       </c>
       <c r="E5" s="54" t="n">
-        <v>291.26</v>
+        <v>271.54</v>
       </c>
       <c r="F5" s="54" t="n">
-        <v>292.1783</v>
+        <v>273.3012</v>
       </c>
       <c r="G5" s="54" t="n">
-        <v>287.17</v>
+        <v>265.89</v>
       </c>
       <c r="H5" s="54" t="n">
-        <v>288.37</v>
+        <v>272.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added environment variable for TD_ACCOUNT
</commit_message>
<xml_diff>
--- a/excelworkbooktest/TD Ameritrade stonks.xlsx
+++ b/excelworkbooktest/TD Ameritrade stonks.xlsx
@@ -358,9 +358,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="4"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
       <alignment horizontal="center"/>
     </xf>
@@ -993,11 +993,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:IT254"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E11" sqref="E11"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -1083,7 +1083,7 @@
         <v/>
       </c>
       <c r="F2" s="43" t="n">
-        <v>32966.58</v>
+        <v>33260.64</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(F2-E2) / E2</f>
@@ -1256,6 +1256,8 @@
         <v/>
       </c>
     </row>
+    <row r="9"/>
+    <row r="10"/>
     <row r="11">
       <c r="D11">
         <f>IF(A11="","",SUM(F11*B11))</f>
@@ -1345,6 +1347,239 @@
       <c r="M21" s="45" t="n"/>
       <c r="O21" s="45" t="n"/>
     </row>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230"/>
+    <row r="231"/>
+    <row r="232"/>
+    <row r="233"/>
+    <row r="234"/>
+    <row r="235"/>
+    <row r="236"/>
+    <row r="237"/>
+    <row r="238"/>
+    <row r="239"/>
+    <row r="240"/>
+    <row r="241"/>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244"/>
+    <row r="245"/>
+    <row r="246"/>
+    <row r="247"/>
+    <row r="248"/>
+    <row r="249"/>
+    <row r="250"/>
+    <row r="251"/>
+    <row r="252"/>
+    <row r="253"/>
+    <row r="254"/>
   </sheetData>
   <conditionalFormatting sqref="G5:G9">
     <cfRule type="dataBar" priority="10">
@@ -1411,8 +1646,8 @@
     <col width="16.453125" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
     <col width="18.81640625" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
     <col width="13.08984375" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
-    <col width="8.7265625" customWidth="1" style="2" min="12" max="75"/>
-    <col width="8.7265625" customWidth="1" style="2" min="76" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="12" max="76"/>
+    <col width="8.7265625" customWidth="1" style="2" min="77" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1495,7 +1730,7 @@
         <v/>
       </c>
       <c r="I2" s="28" t="n">
-        <v>32966.58</v>
+        <v>33260.64</v>
       </c>
       <c r="J2" s="29">
         <f>(I2-D2-H2)/D2</f>
@@ -3005,25 +3240,25 @@
         </is>
       </c>
       <c r="B2" s="55" t="n">
-        <v>227.84</v>
+        <v>230.6</v>
       </c>
       <c r="C2" s="55" t="n">
-        <v>228.24</v>
+        <v>230.62</v>
       </c>
       <c r="D2" s="55" t="n">
-        <v>227.8</v>
+        <v>230.618</v>
       </c>
       <c r="E2" s="55" t="n">
-        <v>225.27</v>
+        <v>229.86</v>
       </c>
       <c r="F2" s="55" t="n">
-        <v>228.05</v>
+        <v>230.86</v>
       </c>
       <c r="G2" s="55" t="n">
-        <v>224.48</v>
+        <v>229.595</v>
       </c>
       <c r="H2" s="55" t="n">
-        <v>225.5</v>
+        <v>227.57</v>
       </c>
     </row>
     <row r="3">
@@ -3033,25 +3268,25 @@
         </is>
       </c>
       <c r="B3" s="55" t="n">
-        <v>415.11</v>
+        <v>419.62</v>
       </c>
       <c r="C3" s="55" t="n">
-        <v>415.19</v>
+        <v>419.64</v>
       </c>
       <c r="D3" s="55" t="n">
-        <v>415.13</v>
+        <v>419.61</v>
       </c>
       <c r="E3" s="55" t="n">
-        <v>410.72</v>
+        <v>418.55</v>
       </c>
       <c r="F3" s="55" t="n">
-        <v>415.46</v>
+        <v>420.17</v>
       </c>
       <c r="G3" s="55" t="n">
-        <v>409.35</v>
+        <v>418.345</v>
       </c>
       <c r="H3" s="55" t="n">
-        <v>411.16</v>
+        <v>414.49</v>
       </c>
     </row>
     <row r="4">
@@ -3061,25 +3296,25 @@
         </is>
       </c>
       <c r="B4" s="55" t="n">
-        <v>451.55</v>
+        <v>456.42</v>
       </c>
       <c r="C4" s="55" t="n">
-        <v>451.6</v>
+        <v>456.43</v>
       </c>
       <c r="D4" s="55" t="n">
-        <v>451.55</v>
+        <v>456.42</v>
       </c>
       <c r="E4" s="55" t="n">
-        <v>446.73</v>
+        <v>455.22</v>
       </c>
       <c r="F4" s="55" t="n">
-        <v>451.92</v>
+        <v>457.029</v>
       </c>
       <c r="G4" s="55" t="n">
-        <v>445.22</v>
+        <v>455.005</v>
       </c>
       <c r="H4" s="55" t="n">
-        <v>447.26</v>
+        <v>450.94</v>
       </c>
     </row>
     <row r="5">
@@ -3089,25 +3324,25 @@
         </is>
       </c>
       <c r="B5" s="55" t="n">
-        <v>269.92</v>
+        <v>278.98</v>
       </c>
       <c r="C5" s="55" t="n">
-        <v>279.73</v>
+        <v>279.04</v>
       </c>
       <c r="D5" s="55" t="n">
+        <v>279.02</v>
+      </c>
+      <c r="E5" s="55" t="n">
+        <v>278.15</v>
+      </c>
+      <c r="F5" s="55" t="n">
+        <v>279.0591</v>
+      </c>
+      <c r="G5" s="55" t="n">
+        <v>277.48</v>
+      </c>
+      <c r="H5" s="55" t="n">
         <v>274.9</v>
-      </c>
-      <c r="E5" s="55" t="n">
-        <v>271.26</v>
-      </c>
-      <c r="F5" s="55" t="n">
-        <v>275.58</v>
-      </c>
-      <c r="G5" s="55" t="n">
-        <v>270.43</v>
-      </c>
-      <c r="H5" s="55" t="n">
-        <v>272.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>